<commit_message>
Update README and small fixes
</commit_message>
<xml_diff>
--- a/sample_music_url_list.xlsx
+++ b/sample_music_url_list.xlsx
@@ -1,87 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$A$1:$H$1</definedName>
-  </definedNames>
-  <calcPr fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>artist</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>downloaded</t>
-  </si>
-  <si>
-    <t>mark_delete</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=M6PLSJUzo8Q&amp;list=RDGMEMYH9CUrFO7CfLJpaD7UR85w&amp;start_radio=1&amp;rv=BhSbRAoxm7E</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Vpop</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -124,51 +83,113 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -456,69 +477,95 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="8" width="56.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="73.7192857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="19.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="19.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="19.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="19.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="10" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="19.005" customWidth="1" bestFit="1"/>
+    <col width="56.005" bestFit="1" customWidth="1" style="8" min="1" max="1"/>
+    <col width="73.7192857142857" bestFit="1" customWidth="1" style="8" min="2" max="2"/>
+    <col width="19.43357142857143" bestFit="1" customWidth="1" style="9" min="3" max="3"/>
+    <col width="19.43357142857143" bestFit="1" customWidth="1" style="9" min="4" max="4"/>
+    <col width="19.43357142857143" bestFit="1" customWidth="1" style="9" min="5" max="5"/>
+    <col width="19.43357142857143" bestFit="1" customWidth="1" style="9" min="6" max="6"/>
+    <col width="12.14785714285714" bestFit="1" customWidth="1" style="10" min="7" max="7"/>
+    <col width="19.005" bestFit="1" customWidth="1" style="9" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>artist</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>version</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>category</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>downloaded</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>mark_delete</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="44.25" customHeight="1">
+      <c r="A2" s="4" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=M6PLSJUzo8Q&amp;list=RDGMEMYH9CUrFO7CfLJpaD7UR85w&amp;start_radio=1&amp;rv=BhSbRAoxm7E</t>
+        </is>
+      </c>
+      <c r="B2" s="5" t="inlineStr">
+        <is>
+          <t>JUSTATEE x PHƯƠNG LY - THẰNG ĐIÊN ( Speed Up )</t>
+        </is>
+      </c>
+      <c r="C2" s="9" t="n"/>
+      <c r="D2" s="9" t="n"/>
+      <c r="E2" s="9" t="n"/>
+      <c r="F2" s="9" t="inlineStr">
+        <is>
+          <t>Vpop</t>
+        </is>
+      </c>
+      <c r="G2" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="44.25">
-      <c r="A2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="6"/>
+      <c r="H2" s="9" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>